<commit_message>
Error and Message Table
ตาราง Error กับ Message
</commit_message>
<xml_diff>
--- a/Error and message Table.xlsx
+++ b/Error and message Table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2015-1\SW En\ProjectCPEform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\คุณจริยา ศรีเอี่ยม\Desktop\FormCPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,9 +24,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Error Tabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -63,8 +135,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,18 +426,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>